<commit_message>
faltando edicao de registros
</commit_message>
<xml_diff>
--- a/excel/IMDB.xlsx
+++ b/excel/IMDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\MovieShuffle\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FC64B7-0AF6-4D5D-9F47-44FCC6E84734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78867EAE-DF62-4CA7-A636-B32D340A9577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E0ABBC8E-8120-4144-B467-A69213250907}"/>
   </bookViews>
@@ -1178,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A6D0D53-FAC2-4D83-B698-A1A7FF06ADAA}">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>

</xml_diff>